<commit_message>
Cox Exploration build up
</commit_message>
<xml_diff>
--- a/results/tabla_4a_raw.xlsx
+++ b/results/tabla_4a_raw.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+  <si>
+    <t>Predictor</t>
+  </si>
   <si>
     <t>aHR</t>
   </si>
@@ -410,13 +413,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,149 +444,167 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
         <v>0.9896912698857327</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.9546935188103011</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.025971990370933</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.5726767769483435</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>-0.01036223308865754</v>
       </c>
-      <c r="G2">
-        <v>-0.04636491271984701</v>
-      </c>
       <c r="H2">
+        <v>-0.046364912719847</v>
+      </c>
+      <c r="I2">
         <v>0.02564044654253193</v>
       </c>
-      <c r="I2">
-        <v>0.01836905163318001</v>
+      <c r="J2">
+        <v>0.01836905163318</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
         <v>1.177578032477161</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1.080303167872079</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1.283611919146925</v>
       </c>
-      <c r="E3">
-        <v>0.0002025048343967594</v>
-      </c>
       <c r="F3">
-        <v>0.163459814332371</v>
+        <v>0.0002025048343967579</v>
       </c>
       <c r="G3">
-        <v>0.07724171273683486</v>
+        <v>0.1634598143323711</v>
       </c>
       <c r="H3">
+        <v>0.07724171273683492</v>
+      </c>
+      <c r="I3">
         <v>0.2496779159279072</v>
       </c>
-      <c r="I3">
-        <v>0.04398963566453953</v>
+      <c r="J3">
+        <v>0.04398963566453952</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>0.7034266303779289</v>
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>0.09619852309113185</v>
+        <v>0.7034266303779287</v>
       </c>
       <c r="D4">
-        <v>5.143623918800701</v>
+        <v>0.0961985230911318</v>
       </c>
       <c r="E4">
+        <v>5.1436239188007</v>
+      </c>
+      <c r="F4">
         <v>0.7289216131112743</v>
       </c>
-      <c r="F4">
-        <v>-0.3517917001509057</v>
-      </c>
       <c r="G4">
+        <v>-0.3517917001509059</v>
+      </c>
+      <c r="H4">
         <v>-2.341341273911364</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1.637757873609552</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1.015094965751295</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
         <v>0.4252064290016825</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.1922082177657556</v>
       </c>
-      <c r="D5">
-        <v>0.9406492051484743</v>
-      </c>
       <c r="E5">
-        <v>0.03477247702194703</v>
+        <v>0.9406492051484744</v>
       </c>
       <c r="F5">
-        <v>-0.8551805126811365</v>
+        <v>0.03477247702194716</v>
       </c>
       <c r="G5">
+        <v>-0.8551805126811364</v>
+      </c>
+      <c r="H5">
         <v>-1.649176027034499</v>
       </c>
-      <c r="H5">
-        <v>-0.0611849983277738</v>
-      </c>
       <c r="I5">
+        <v>-0.06118499832777369</v>
+      </c>
+      <c r="J5">
         <v>0.4051071961608979</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>0.5975640541401354</v>
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
       <c r="C6">
+        <v>0.5975640541401352</v>
+      </c>
+      <c r="D6">
         <v>0.2299967188385167</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>1.552556056467512</v>
       </c>
-      <c r="E6">
-        <v>0.2905338324226386</v>
-      </c>
       <c r="F6">
-        <v>-0.5148937973405482</v>
+        <v>0.2905338324226384</v>
       </c>
       <c r="G6">
-        <v>-1.469690236080193</v>
+        <v>-0.5148937973405483</v>
       </c>
       <c r="H6">
-        <v>0.439902641399097</v>
+        <v>-1.469690236080194</v>
       </c>
       <c r="I6">
+        <v>0.4399026413990968</v>
+      </c>
+      <c r="J6">
         <v>0.4871499916687029</v>
       </c>
     </row>

</xml_diff>